<commit_message>
Added partial list of Digikey part numbers.
</commit_message>
<xml_diff>
--- a/RTx_Manual_Control/RTxManualControlBOM.xlsx
+++ b/RTx_Manual_Control/RTxManualControlBOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="60">
   <si>
     <t>Qty</t>
   </si>
@@ -151,6 +151,51 @@
   </si>
   <si>
     <t>PIN HEADER POLARIZED</t>
+  </si>
+  <si>
+    <t>311-1376-1-ND</t>
+  </si>
+  <si>
+    <t>Order Qty</t>
+  </si>
+  <si>
+    <t>311-1181-1-ND</t>
+  </si>
+  <si>
+    <t>311-10.0KFRCT-ND</t>
+  </si>
+  <si>
+    <t>311-1.00KFRCT-ND</t>
+  </si>
+  <si>
+    <t>311-280FRCT-ND</t>
+  </si>
+  <si>
+    <t>311-620FRCT-ND</t>
+  </si>
+  <si>
+    <t>609-3406-ND</t>
+  </si>
+  <si>
+    <t>Female-1X6</t>
+  </si>
+  <si>
+    <t>Female-1X8</t>
+  </si>
+  <si>
+    <t>Female-1X2</t>
+  </si>
+  <si>
+    <t>Female-1X6 Polarized</t>
+  </si>
+  <si>
+    <t>Female-2X3 Polarized</t>
+  </si>
+  <si>
+    <t>Female-1X3 Polarized</t>
+  </si>
+  <si>
+    <t>A106652-ND</t>
   </si>
 </sst>
 </file>
@@ -513,26 +558,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="54.5703125" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="54.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10" ht="29.25">
       <c r="A1" s="3" t="s">
         <v>35</v>
       </c>
@@ -540,278 +586,416 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" ht="17.25" customHeight="1">
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" ht="17.25" customHeight="1">
       <c r="B2" s="2">
         <v>7</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="2">
+        <v>21</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" ht="17.25" customHeight="1">
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" ht="17.25" customHeight="1">
       <c r="B3" s="2">
         <v>3</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="4" t="s">
+      <c r="C3" s="2">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" ht="17.25" customHeight="1">
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" ht="17.25" customHeight="1">
       <c r="B4" s="2">
         <v>3</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="4" t="s">
+      <c r="C4" s="2">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" ht="17.25" customHeight="1">
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" ht="17.25" customHeight="1">
       <c r="B5" s="2">
         <v>3</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="4" t="s">
+      <c r="C5" s="2">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" ht="17.25" customHeight="1">
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" ht="17.25" customHeight="1">
       <c r="B6" s="2">
         <v>6</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="4">
+      <c r="C6" s="2">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="4">
         <v>280</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" ht="17.25" customHeight="1">
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" ht="17.25" customHeight="1">
       <c r="B7" s="2">
         <v>4</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="4">
+      <c r="C7" s="2">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="4">
         <v>620</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" ht="17.25" customHeight="1">
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" ht="17.25" customHeight="1">
       <c r="B8" s="2">
         <v>2</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="2" t="s">
+      <c r="C8" s="2">
+        <v>6</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" ht="17.25" customHeight="1">
-      <c r="B9" s="2">
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" ht="17.25" customHeight="1">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" ht="17.25" customHeight="1">
+      <c r="B10" s="2">
         <v>2</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="2" t="s">
+      <c r="C10" s="2">
+        <v>6</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" ht="17.25" customHeight="1">
-      <c r="B10" s="2">
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" ht="17.25" customHeight="1">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2">
+        <v>6</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" ht="17.25" customHeight="1">
+      <c r="B12" s="2">
         <v>1</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="4" t="s">
+      <c r="C12" s="2">
+        <v>3</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" ht="17.25" customHeight="1">
-      <c r="B11" s="2">
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" ht="17.25" customHeight="1">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2">
+        <v>3</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" ht="17.25" customHeight="1">
+      <c r="B14" s="2">
         <v>2</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="2" t="s">
+      <c r="C14" s="2">
+        <v>6</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" ht="17.25" customHeight="1">
-      <c r="B12" s="2">
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" ht="17.25" customHeight="1">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2">
+        <v>6</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" ht="17.25" customHeight="1">
+      <c r="B16" s="2">
         <v>2</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="2" t="s">
+      <c r="C16" s="2">
+        <v>6</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="G16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="I16" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" ht="17.25" customHeight="1">
-      <c r="B13" s="2">
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="2:10" ht="17.25" customHeight="1">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2">
+        <v>6</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+    </row>
+    <row r="18" spans="2:10" ht="17.25" customHeight="1">
+      <c r="B18" s="2">
         <v>1</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="4" t="s">
+      <c r="C18" s="2">
+        <v>3</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="G18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="H18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="I18" s="2" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10">
+      <c r="C19" s="2">
+        <v>3</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added headers/socket part numbers.
</commit_message>
<xml_diff>
--- a/RTx_Manual_Control/RTxManualControlBOM.xlsx
+++ b/RTx_Manual_Control/RTxManualControlBOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="70">
   <si>
     <t>Qty</t>
   </si>
@@ -195,7 +195,37 @@
     <t>Female-1X3 Polarized</t>
   </si>
   <si>
-    <t>A106652-ND</t>
+    <t>S7039-ND</t>
+  </si>
+  <si>
+    <t>S7041-ND</t>
+  </si>
+  <si>
+    <t>S9414-ND</t>
+  </si>
+  <si>
+    <t>SWR25X</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>SWH25X</t>
+  </si>
+  <si>
+    <t>S9436-ND</t>
+  </si>
+  <si>
+    <t>S9434-ND</t>
+  </si>
+  <si>
+    <t>S9435-ND</t>
+  </si>
+  <si>
+    <t>S9411-ND</t>
+  </si>
+  <si>
+    <t>S9407-ND</t>
   </si>
 </sst>
 </file>
@@ -252,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -263,6 +293,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -558,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -570,15 +609,16 @@
     <col min="2" max="2" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5703125" customWidth="1"/>
     <col min="4" max="4" width="25.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="54.5703125" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="7" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="54.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="29.25">
+    <row r="1" spans="1:11" ht="29.25">
       <c r="A1" s="3" t="s">
         <v>35</v>
       </c>
@@ -591,24 +631,27 @@
       <c r="D1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:10" ht="17.25" customHeight="1">
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" ht="17.25" customHeight="1">
       <c r="B2" s="2">
         <v>7</v>
       </c>
@@ -618,24 +661,25 @@
       <c r="D2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" ht="17.25" customHeight="1">
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" ht="17.25" customHeight="1">
       <c r="B3" s="2">
         <v>3</v>
       </c>
@@ -645,24 +689,25 @@
       <c r="D3" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="6"/>
+      <c r="F3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" ht="17.25" customHeight="1">
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" ht="17.25" customHeight="1">
       <c r="B4" s="2">
         <v>3</v>
       </c>
@@ -672,24 +717,25 @@
       <c r="D4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="6"/>
+      <c r="F4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" ht="17.25" customHeight="1">
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:11" ht="17.25" customHeight="1">
       <c r="B5" s="2">
         <v>3</v>
       </c>
@@ -699,24 +745,25 @@
       <c r="D5" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="6"/>
+      <c r="F5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" ht="17.25" customHeight="1">
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:11" ht="17.25" customHeight="1">
       <c r="B6" s="2">
         <v>6</v>
       </c>
@@ -726,24 +773,25 @@
       <c r="D6" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="6"/>
+      <c r="F6" s="4">
         <v>280</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" ht="17.25" customHeight="1">
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" ht="17.25" customHeight="1">
       <c r="B7" s="2">
         <v>4</v>
       </c>
@@ -753,24 +801,25 @@
       <c r="D7" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="6"/>
+      <c r="F7" s="4">
         <v>620</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:10" ht="17.25" customHeight="1">
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" ht="17.25" customHeight="1">
       <c r="B8" s="2">
         <v>2</v>
       </c>
@@ -780,37 +829,39 @@
       <c r="D8" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="2" t="s">
+      <c r="E8" s="6"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" ht="17.25" customHeight="1">
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" ht="17.25" customHeight="1">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="2" t="s">
+      <c r="E9" s="6"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" ht="17.25" customHeight="1">
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" ht="17.25" customHeight="1">
       <c r="B10" s="2">
         <v>2</v>
       </c>
@@ -820,115 +871,134 @@
       <c r="D10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="2" t="s">
+      <c r="E10" s="6"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="J10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" ht="17.25" customHeight="1">
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" ht="17.25" customHeight="1">
       <c r="B11" s="2"/>
       <c r="C11" s="2">
         <v>6</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="2" t="s">
+      <c r="D11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" ht="17.25" customHeight="1">
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" ht="17.25" customHeight="1">
       <c r="B12" s="2">
         <v>1</v>
       </c>
       <c r="C12" s="2">
         <v>3</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="4" t="s">
+      <c r="D12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="J12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" ht="17.25" customHeight="1">
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" ht="17.25" customHeight="1">
       <c r="B13" s="2"/>
       <c r="C13" s="2">
         <v>3</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="2" t="s">
+      <c r="D13" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" ht="17.25" customHeight="1">
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" ht="17.25" customHeight="1">
       <c r="B14" s="2">
         <v>2</v>
       </c>
       <c r="C14" s="2">
         <v>6</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="2" t="s">
+      <c r="D14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="J14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" ht="17.25" customHeight="1">
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" ht="17.25" customHeight="1">
       <c r="B15" s="2"/>
       <c r="C15" s="2">
         <v>6</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="2" t="s">
+      <c r="D15" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" ht="17.25" customHeight="1">
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" ht="17.25" customHeight="1">
       <c r="B16" s="2">
         <v>2</v>
       </c>
@@ -936,65 +1006,78 @@
         <v>6</v>
       </c>
       <c r="D16" s="2"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="2" t="s">
+      <c r="E16" s="6"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="H16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="I16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="J16" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="2:10" ht="17.25" customHeight="1">
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="2:11" ht="17.25" customHeight="1">
       <c r="B17" s="2"/>
       <c r="C17" s="2">
         <v>6</v>
       </c>
       <c r="D17" s="2"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="2" t="s">
+      <c r="E17" s="6"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
-    </row>
-    <row r="18" spans="2:10" ht="17.25" customHeight="1">
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="2:11" ht="17.25" customHeight="1">
       <c r="B18" s="2">
         <v>1</v>
       </c>
       <c r="C18" s="2">
         <v>3</v>
       </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="4" t="s">
+      <c r="D18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="G18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="H18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="I18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="J18" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="2:10">
+    <row r="19" spans="2:11">
       <c r="C19" s="2">
         <v>3</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="D19" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>58</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Completed RTxManualControlBOM.xlsx for order.
</commit_message>
<xml_diff>
--- a/RTx_Manual_Control/RTxManualControlBOM.xlsx
+++ b/RTx_Manual_Control/RTxManualControlBOM.xlsx
@@ -8,15 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="72">
   <si>
     <t>Qty</t>
   </si>
@@ -226,13 +224,19 @@
   </si>
   <si>
     <t>S9407-ND</t>
+  </si>
+  <si>
+    <t>609-2841-ND</t>
+  </si>
+  <si>
+    <t>609-2845-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,6 +265,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -282,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -303,6 +313,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,20 +610,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" style="7" customWidth="1"/>
-    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="54.5703125" customWidth="1"/>
@@ -623,25 +634,25 @@
         <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
@@ -653,23 +664,23 @@
     </row>
     <row r="2" spans="1:11" ht="17.25" customHeight="1">
       <c r="B2" s="2">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="2">
         <v>7</v>
-      </c>
-      <c r="C2" s="2">
-        <v>21</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>14</v>
@@ -681,23 +692,23 @@
     </row>
     <row r="3" spans="1:11" ht="17.25" customHeight="1">
       <c r="B3" s="2">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="2">
         <v>3</v>
-      </c>
-      <c r="C3" s="2">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>19</v>
@@ -709,23 +720,23 @@
     </row>
     <row r="4" spans="1:11" ht="17.25" customHeight="1">
       <c r="B4" s="2">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="2">
         <v>3</v>
-      </c>
-      <c r="C4" s="2">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>9</v>
@@ -737,23 +748,23 @@
     </row>
     <row r="5" spans="1:11" ht="17.25" customHeight="1">
       <c r="B5" s="2">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="2">
         <v>3</v>
-      </c>
-      <c r="C5" s="2">
-        <v>10</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>17</v>
@@ -765,23 +776,23 @@
     </row>
     <row r="6" spans="1:11" ht="17.25" customHeight="1">
       <c r="B6" s="2">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="4">
+        <v>280</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="2">
         <v>6</v>
-      </c>
-      <c r="C6" s="2">
-        <v>18</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="4">
-        <v>280</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>20</v>
@@ -793,23 +804,23 @@
     </row>
     <row r="7" spans="1:11" ht="17.25" customHeight="1">
       <c r="B7" s="2">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="4">
+        <v>620</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="2">
         <v>4</v>
-      </c>
-      <c r="C7" s="2">
-        <v>12</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="4">
-        <v>620</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>21</v>
@@ -821,21 +832,21 @@
     </row>
     <row r="8" spans="1:11" ht="17.25" customHeight="1">
       <c r="B8" s="2">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="2">
         <v>2</v>
-      </c>
-      <c r="C8" s="2">
-        <v>6</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>37</v>
@@ -846,16 +857,18 @@
       <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:11" ht="17.25" customHeight="1">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2" t="s">
+      <c r="B9" s="2">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="2" t="s">
+      <c r="D9" s="6"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -863,21 +876,21 @@
     </row>
     <row r="10" spans="1:11" ht="17.25" customHeight="1">
       <c r="B10" s="2">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="2">
         <v>2</v>
-      </c>
-      <c r="C10" s="2">
-        <v>6</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>38</v>
@@ -888,18 +901,18 @@
       <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:11" ht="17.25" customHeight="1">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2">
+      <c r="B11" s="2">
         <v>6</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="2" t="s">
+      <c r="D11" s="6"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -907,23 +920,23 @@
     </row>
     <row r="12" spans="1:11" ht="17.25" customHeight="1">
       <c r="B12" s="2">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="2">
         <v>1</v>
-      </c>
-      <c r="C12" s="2">
-        <v>3</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>31</v>
@@ -934,18 +947,18 @@
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:11" ht="17.25" customHeight="1">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2">
+      <c r="B13" s="2">
         <v>3</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="2" t="s">
+      <c r="D13" s="6"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -953,22 +966,22 @@
     </row>
     <row r="14" spans="1:11" ht="17.25" customHeight="1">
       <c r="B14" s="2">
+        <v>6</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" s="2">
         <v>2</v>
-      </c>
-      <c r="C14" s="2">
-        <v>6</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>43</v>
@@ -979,20 +992,20 @@
       <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:11" ht="17.25" customHeight="1">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2">
+      <c r="B15" s="2">
         <v>6</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="D15" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="2" t="s">
+      <c r="E15" s="4"/>
+      <c r="F15" s="2" t="s">
         <v>56</v>
       </c>
+      <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -1000,19 +1013,21 @@
     </row>
     <row r="16" spans="1:11" ht="17.25" customHeight="1">
       <c r="B16" s="2">
+        <v>6</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="2">
         <v>2</v>
-      </c>
-      <c r="C16" s="2">
-        <v>6</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>42</v>
@@ -1023,16 +1038,18 @@
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="2:11" ht="17.25" customHeight="1">
-      <c r="B17" s="2"/>
-      <c r="C17" s="2">
+      <c r="B17" s="2">
         <v>6</v>
       </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="2" t="s">
+      <c r="C17" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="2" t="s">
         <v>57</v>
       </c>
+      <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -1040,25 +1057,25 @@
     </row>
     <row r="18" spans="2:11" ht="17.25" customHeight="1">
       <c r="B18" s="2">
+        <v>3</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" s="2">
         <v>1</v>
-      </c>
-      <c r="C18" s="2">
-        <v>3</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>34</v>
@@ -1068,16 +1085,16 @@
       </c>
     </row>
     <row r="19" spans="2:11">
-      <c r="C19" s="2">
+      <c r="B19" s="2">
         <v>3</v>
       </c>
-      <c r="D19" t="s">
+      <c r="C19" t="s">
         <v>66</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="D19" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1085,28 +1102,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>